<commit_message>
fixed: Bug #2023080101 调整模版文件表头
</commit_message>
<xml_diff>
--- a/template/amazon.xlsx
+++ b/template/amazon.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="107">
   <si>
     <t>European Amazon Declared Value-Analysis Report(v2.0)</t>
   </si>
@@ -72,16 +72,16 @@
     <t>Profit</t>
   </si>
   <si>
-    <t>NL LOCAL Cost(Euro/ KG)</t>
+    <t>LOCAL Cost(Euro/ KG)</t>
   </si>
   <si>
     <t xml:space="preserve"> Rate + freight outside EU incl Duty (In Euro)</t>
   </si>
   <si>
-    <t>Customs Value includes freight cost occurred outside EU-NL (In Euro)</t>
-  </si>
-  <si>
-    <t>NL Duty</t>
+    <t>Customs Value includes freight cost occurred outside EU(In Euro)</t>
+  </si>
+  <si>
+    <t>Duty</t>
   </si>
   <si>
     <t>Total Customs Value</t>
@@ -186,13 +186,13 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>NL Duty Rate</t>
-  </si>
-  <si>
-    <t>NL Duty Rate(%)</t>
-  </si>
-  <si>
-    <t>NL Duty Amount</t>
+    <t>Duty Rate</t>
+  </si>
+  <si>
+    <t>Duty Rate(%)</t>
+  </si>
+  <si>
+    <t>Duty Amount</t>
   </si>
   <si>
     <t>Information Source</t>
@@ -400,16 +400,34 @@
     <t xml:space="preserve">                                                                   Powered by</t>
   </si>
   <si>
-    <t>ASL Dutch</t>
+    <t>ASL</t>
   </si>
   <si>
     <t>European Amazon Declared Value-Analysis Report</t>
   </si>
   <si>
+    <t>NL LOCAL Cost(Euro/ KG)</t>
+  </si>
+  <si>
+    <t>Customs Value includes freight cost occurred outside EU-NL (In Euro)</t>
+  </si>
+  <si>
+    <t>NL Duty</t>
+  </si>
+  <si>
     <t>Ground Sercice Rate</t>
   </si>
   <si>
     <t>Ground Sercice Fee</t>
+  </si>
+  <si>
+    <t>NL Duty Rate</t>
+  </si>
+  <si>
+    <t>NL Duty Rate(%)</t>
+  </si>
+  <si>
+    <t>NL Duty Amount</t>
   </si>
   <si>
     <t>AsinCode</t>
@@ -433,16 +451,16 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="11">
     <numFmt numFmtId="176" formatCode="0.000000"/>
-    <numFmt numFmtId="177" formatCode="#,##0&quot; &quot;"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="179" formatCode="0.00000000&quot; &quot;"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00&quot; &quot;"/>
+    <numFmt numFmtId="178" formatCode="0.00000000&quot; &quot;"/>
+    <numFmt numFmtId="179" formatCode="0.00&quot; &quot;"/>
+    <numFmt numFmtId="180" formatCode="#,##0&quot; &quot;"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="0.0000"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="0.000"/>
-    <numFmt numFmtId="181" formatCode="#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="182" formatCode="0.00&quot; &quot;"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="0.000"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -491,7 +509,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -499,6 +517,59 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,71 +583,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,23 +607,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -627,6 +621,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
@@ -634,10 +643,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -681,19 +699,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,13 +717,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,96 +735,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -831,7 +747,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,19 +849,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,11 +1045,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,6 +1074,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,24 +1110,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,177 +1142,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1295,7 +1313,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1304,11 +1322,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1316,6 +1331,9 @@
     <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1328,7 +1346,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,16 +1400,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="182" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="182" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1400,24 +1418,24 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3054,7 +3072,7 @@
   <dimension ref="A1:BA26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83035714285714" defaultRowHeight="14" customHeight="1"/>
@@ -5024,7 +5042,7 @@
       </c>
       <c r="AJ3" s="7"/>
       <c r="AK3" s="6" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="AL3" s="7"/>
       <c r="AM3" s="7"/>
@@ -5040,10 +5058,10 @@
         <v>19</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
@@ -5135,10 +5153,10 @@
         <v>17</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="AL4" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AM4" s="6" t="s">
         <v>47</v>
@@ -5170,13 +5188,13 @@
       <c r="AV4" s="7"/>
       <c r="AW4" s="7"/>
       <c r="AX4" s="6" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="AY4" s="21" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="AZ4" s="6" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="BA4" s="31"/>
     </row>
@@ -5185,10 +5203,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D5" s="10">
         <v>1</v>
@@ -5214,13 +5232,13 @@
         <v>0</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="N5" s="19">
         <v>0</v>

</xml_diff>